<commit_message>
property reader class added
</commit_message>
<xml_diff>
--- a/src/test/resources/files/SampleExcel.xlsx
+++ b/src/test/resources/files/SampleExcel.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>username</t>
   </si>
@@ -130,10 +130,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>

</xml_diff>